<commit_message>
added all files till 15/05/25
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestdata.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM5thDecWorkSpace\DataAndKeyDrivenTesting\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3AF0AD0-EC70-4E07-B792-2EA3A76619AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2E693C4-4A23-467D-963E-CE929CFD1490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D0288085-FE06-45FF-BB2A-5DF0CCBCF2C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="testdata" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Sashikumar</t>
   </si>
   <si>
-    <t>sashikumar@47</t>
-  </si>
-  <si>
     <t>TC-002</t>
   </si>
   <si>
@@ -57,7 +54,82 @@
     <t>Adactin.com - Hotel Reservation System</t>
   </si>
   <si>
-    <t>Sashikumaasfdgr</t>
+    <t>Sashikumar@47</t>
+  </si>
+  <si>
+    <t>TC-004</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>Hotel</t>
+  </si>
+  <si>
+    <t>Hotel Creek</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Check In Date</t>
+  </si>
+  <si>
+    <t>Check Out Date</t>
+  </si>
+  <si>
+    <t>Check-Out Date shall be after than Check-In Date</t>
+  </si>
+  <si>
+    <t>Room Type</t>
+  </si>
+  <si>
+    <t>TC-003</t>
+  </si>
+  <si>
+    <t>ConfirmPassword</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>EmailAddress</t>
+  </si>
+  <si>
+    <t>KumarSSLK</t>
+  </si>
+  <si>
+    <t>kumar@gmail.com</t>
+  </si>
+  <si>
+    <t>catcha</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>kumar@1234</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Adactin.com - New User Registration</t>
+  </si>
+  <si>
+    <t>TC-005</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>hotel</t>
+  </si>
+  <si>
+    <t>roomtype</t>
   </si>
 </sst>
 </file>
@@ -102,9 +174,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,20 +494,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14621E4-C4E7-4004-A2AF-5A088D5705FD}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.21875" customWidth="1"/>
     <col min="4" max="4" width="34.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -447,7 +527,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -455,15 +535,15 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>0</v>
@@ -475,46 +555,174 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="2">
+        <v>45798</v>
+      </c>
+      <c r="H11" s="2">
+        <v>45792</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C14" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="1" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -523,8 +731,14 @@
     <hyperlink ref="D2" r:id="rId2" display="https://adactinhotelapp.com/" xr:uid="{53A00CDE-7506-4A8E-9C95-C34AD1FEE87D}"/>
     <hyperlink ref="C5" r:id="rId3" xr:uid="{E8E4CA86-CF7F-4B45-B39E-C70AC1BCAA0F}"/>
     <hyperlink ref="D5" r:id="rId4" display="https://adactinhotelapp.com/" xr:uid="{6AC80E97-97DF-4301-8807-5A458A89ABCF}"/>
-    <hyperlink ref="C8" r:id="rId5" xr:uid="{8EAE50EF-CBF5-4D98-BAF9-3A30D26A0773}"/>
-    <hyperlink ref="D8" r:id="rId6" display="https://adactinhotelapp.com/" xr:uid="{D88E1C49-E7AE-4977-842F-DC98F399A277}"/>
+    <hyperlink ref="B8" r:id="rId5" display="https://adactinhotelapp.com/" xr:uid="{D88E1C49-E7AE-4977-842F-DC98F399A277}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{6C28804A-FD9F-4CE0-ADEE-73E9E344F921}"/>
+    <hyperlink ref="I11" r:id="rId7" display="https://adactinhotelapp.com/" xr:uid="{936859DB-0048-42D1-B5DC-B67F0EDE2B5D}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{12E6FE2C-64B0-4869-B627-091D474393FD}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{C841870F-BBF2-441C-9A82-B82F9EF2E2A8}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{BD7D10E1-51EB-4061-9364-D2D93F9CA07F}"/>
+    <hyperlink ref="C15" r:id="rId11" xr:uid="{999EA241-49DF-4A16-ABBC-DE5A76A38863}"/>
+    <hyperlink ref="G15" r:id="rId12" display="https://adactinhotelapp.com/" xr:uid="{D7C16B8A-3B40-4DAB-B346-1816316732F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>